<commit_message>
student and teacher database table added to design
</commit_message>
<xml_diff>
--- a/Documentation/Database Details/Database Mockup Design.xlsx
+++ b/Documentation/Database Details/Database Mockup Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>Admin Table</t>
   </si>
@@ -29,13 +29,25 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>Teacher Table</t>
+  </si>
+  <si>
+    <t>Student Table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,8 +71,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -72,8 +107,14 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -96,21 +137,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -412,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D4"/>
+  <dimension ref="A3:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,30 +485,106 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
class table, quiz table, student_quiz table and quiz_question table added to database design
</commit_message>
<xml_diff>
--- a/Documentation/Database Details/Database Mockup Design.xlsx
+++ b/Documentation/Database Details/Database Mockup Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Admin Table</t>
   </si>
@@ -41,6 +41,81 @@
   </si>
   <si>
     <t>Student Table</t>
+  </si>
+  <si>
+    <t>Classroom Table</t>
+  </si>
+  <si>
+    <t>created_by</t>
+  </si>
+  <si>
+    <t>class_code</t>
+  </si>
+  <si>
+    <t>created_date</t>
+  </si>
+  <si>
+    <t>Quiz Table</t>
+  </si>
+  <si>
+    <t>classroom_id</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>quiz_type</t>
+  </si>
+  <si>
+    <t>total_marks</t>
+  </si>
+  <si>
+    <t>total_time</t>
+  </si>
+  <si>
+    <t>quiz_timeline</t>
+  </si>
+  <si>
+    <t>quiz_date</t>
+  </si>
+  <si>
+    <t>Student_Quiz_record Table</t>
+  </si>
+  <si>
+    <t>quiz_id</t>
+  </si>
+  <si>
+    <t>obtained_marks</t>
+  </si>
+  <si>
+    <t>obtained_grade</t>
+  </si>
+  <si>
+    <t>correct_answers</t>
+  </si>
+  <si>
+    <t>wrong_answers</t>
+  </si>
+  <si>
+    <t>Quiz_question_record Table</t>
+  </si>
+  <si>
+    <t>question_type</t>
+  </si>
+  <si>
+    <t>question_mark</t>
+  </si>
+  <si>
+    <t>correct_answer</t>
+  </si>
+  <si>
+    <t>question_definition</t>
+  </si>
+  <si>
+    <t>student_id</t>
+  </si>
+  <si>
+    <t>question_number</t>
   </si>
 </sst>
 </file>
@@ -160,12 +235,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -472,119 +547,298 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D15"/>
+  <dimension ref="A3:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A33:D33"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>